<commit_message>
Bugfix for missing municipalities
This commit fixes two bugs: One, four municipalities were incorrectly excluded when parsing the raw 2020 data (namely, Bathurst, Campbellton, Dieppe, and Edmunston), and two, Grande-Anse was incorrectly excluded when parsing the 2005 tax base data (this was more of a transcription error fixed by PR #1).

After updating the source code, the data processing Python scripts were rerun to generate the correct data.
</commit_message>
<xml_diff>
--- a/data/data_clean/2005/GNB2005_tax_base.xlsx
+++ b/data/data_clean/2005/GNB2005_tax_base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Municipality</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Grand Manan</t>
+  </si>
+  <si>
+    <t>Grande-Anse</t>
   </si>
   <si>
     <t>Hampton</t>
@@ -2162,80 +2165,80 @@
         <v>48</v>
       </c>
       <c r="B38" s="3">
-        <v>102569700</v>
+        <v>103165300</v>
       </c>
       <c r="C38" s="3">
-        <v>457100</v>
+        <v>552000</v>
       </c>
       <c r="D38" s="3">
-        <v>5542700</v>
+        <v>5635600</v>
       </c>
       <c r="E38" s="3">
-        <v>108569500</v>
+        <v>109352900</v>
       </c>
       <c r="F38" s="3">
         <v>15022300</v>
       </c>
       <c r="G38" s="3">
-        <v>799400</v>
+        <v>866300</v>
       </c>
       <c r="H38" s="3">
         <v>1690700</v>
       </c>
       <c r="I38" s="3">
-        <v>17512400</v>
+        <v>17579300</v>
       </c>
       <c r="J38" s="3">
-        <v>126081900</v>
+        <v>126932200</v>
       </c>
       <c r="K38" s="3">
-        <v>134838100</v>
+        <v>135721850</v>
       </c>
       <c r="L38" s="3">
-        <v>134799014</v>
+        <v>135682764</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" s="3">
-        <v>20854200</v>
+        <v>20258600</v>
       </c>
       <c r="C39" s="3">
-        <v>94900</v>
+        <v>0</v>
       </c>
       <c r="D39" s="3">
-        <v>3699600</v>
+        <v>3606700</v>
       </c>
       <c r="E39" s="3">
-        <v>24648700</v>
+        <v>23865300</v>
       </c>
       <c r="F39" s="3">
         <v>4262700</v>
       </c>
       <c r="G39" s="3">
-        <v>149200</v>
+        <v>82300</v>
       </c>
       <c r="H39" s="3">
         <v>472300</v>
       </c>
       <c r="I39" s="3">
-        <v>4884200</v>
+        <v>4817300</v>
       </c>
       <c r="J39" s="3">
-        <v>29532900</v>
+        <v>28682600</v>
       </c>
       <c r="K39" s="3">
-        <v>31975000</v>
+        <v>31091250</v>
       </c>
       <c r="L39" s="3">
-        <v>31954125</v>
+        <v>31070375</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" s="3">
         <v>142080300</v>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41" s="3">
         <v>26392400</v>
@@ -2311,7 +2314,7 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" s="3">
         <v>37945600</v>
@@ -2349,7 +2352,7 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" s="3">
         <v>24417400</v>
@@ -2387,7 +2390,7 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44" s="3">
         <v>33203600</v>
@@ -2425,7 +2428,7 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="3">
         <v>21556100</v>
@@ -2463,7 +2466,7 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46" s="3">
         <v>130492400</v>
@@ -2501,7 +2504,7 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" s="3">
         <v>57945300</v>
@@ -2539,7 +2542,7 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B48" s="3">
         <v>28916400</v>
@@ -2577,7 +2580,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49" s="3">
         <v>42213000</v>
@@ -2615,7 +2618,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50" s="3">
         <v>47762400</v>
@@ -2653,7 +2656,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51" s="3">
         <v>46473600</v>
@@ -2691,7 +2694,7 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3">
         <v>41965500</v>
@@ -2729,7 +2732,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53" s="3">
         <v>26955300</v>
@@ -2767,7 +2770,7 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54" s="3">
         <v>23770100</v>
@@ -2805,7 +2808,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B55" s="3">
         <v>33715300</v>
@@ -2843,7 +2846,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B56" s="3">
         <v>25508900</v>
@@ -2881,7 +2884,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B57" s="3">
         <v>132037800</v>
@@ -2919,7 +2922,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3">
         <v>46010100</v>
@@ -2957,7 +2960,7 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3">
         <v>45327100</v>
@@ -2995,7 +2998,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B60" s="3">
         <v>18617500</v>
@@ -3033,7 +3036,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B61" s="3">
         <v>59922300</v>
@@ -3071,7 +3074,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B62" s="3">
         <v>64736100</v>
@@ -3109,7 +3112,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B63" s="3">
         <v>34818000</v>
@@ -3147,7 +3150,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B64" s="3">
         <v>13574300</v>
@@ -3185,7 +3188,7 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B65" s="3">
         <v>7648900</v>
@@ -3223,7 +3226,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B66" s="3">
         <v>14197600</v>
@@ -3261,7 +3264,7 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B67" s="3">
         <v>41395200</v>
@@ -3299,7 +3302,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B68" s="3">
         <v>31393000</v>
@@ -3337,7 +3340,7 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B69" s="3">
         <v>11806400</v>
@@ -3375,7 +3378,7 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B70" s="3">
         <v>27515100</v>
@@ -3413,7 +3416,7 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71" s="3">
         <v>22710300</v>
@@ -3451,7 +3454,7 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B72" s="3">
         <v>19967800</v>
@@ -3489,7 +3492,7 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B73" s="3">
         <v>43395800</v>
@@ -3527,7 +3530,7 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B74" s="3">
         <v>6374500</v>
@@ -3565,7 +3568,7 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B75" s="3">
         <v>13215800</v>
@@ -3603,7 +3606,7 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B76" s="3">
         <v>9574800</v>
@@ -3641,7 +3644,7 @@
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B77" s="3">
         <v>28808800</v>
@@ -3679,7 +3682,7 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B78" s="3">
         <v>19131700</v>
@@ -3717,7 +3720,7 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B79" s="3">
         <v>31099900</v>
@@ -3755,7 +3758,7 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B80" s="3">
         <v>9147900</v>
@@ -3793,7 +3796,7 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B81" s="3">
         <v>14673900</v>
@@ -3831,7 +3834,7 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B82" s="3">
         <v>15249100</v>
@@ -3869,7 +3872,7 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B83" s="3">
         <v>5182200</v>
@@ -3907,7 +3910,7 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B84" s="3">
         <v>6990900</v>
@@ -3945,7 +3948,7 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B85" s="3">
         <v>21640300</v>
@@ -3983,7 +3986,7 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B86" s="3">
         <v>36429400</v>
@@ -4021,7 +4024,7 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B87" s="3">
         <v>14790300</v>
@@ -4059,7 +4062,7 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" s="3">
         <v>20686000</v>
@@ -4097,7 +4100,7 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B89" s="3">
         <v>9285800</v>
@@ -4135,7 +4138,7 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B90" s="3">
         <v>9188300</v>
@@ -4173,7 +4176,7 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B91" s="3">
         <v>20072200</v>
@@ -4211,7 +4214,7 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B92" s="3">
         <v>14199500</v>
@@ -4249,7 +4252,7 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B93" s="3">
         <v>19671000</v>
@@ -4287,7 +4290,7 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B94" s="3">
         <v>12153000</v>
@@ -4325,7 +4328,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B95" s="3">
         <v>25666100</v>
@@ -4363,7 +4366,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B96" s="3">
         <v>18864600</v>
@@ -4401,7 +4404,7 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B97" s="3">
         <v>12960100</v>
@@ -4439,7 +4442,7 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B98" s="3">
         <v>5968300</v>
@@ -4477,7 +4480,7 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B99" s="3">
         <v>11399000</v>
@@ -4515,7 +4518,7 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B100" s="3">
         <v>11074900</v>
@@ -4553,7 +4556,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B101" s="3">
         <v>45862600</v>
@@ -4591,7 +4594,7 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B102" s="3">
         <v>35327900</v>
@@ -4629,7 +4632,7 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B103" s="3">
         <v>15334900</v>
@@ -4667,7 +4670,7 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B104" s="3">
         <v>4537900</v>

</xml_diff>

<commit_message>
Bugfix for missing municipalities (#2)
This commit fixes two bugs: One, four municipalities were incorrectly excluded when parsing the raw 2020 data (namely, Bathurst, Campbellton, Dieppe, and Edmunston), and two, Grande-Anse was incorrectly excluded when parsing the 2005 tax base data (this was more of a transcription error fixed by PR #1).

After updating the source code, the data processing Python scripts were rerun to generate the correct data.
</commit_message>
<xml_diff>
--- a/data/data_clean/2005/GNB2005_tax_base.xlsx
+++ b/data/data_clean/2005/GNB2005_tax_base.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Municipality</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Grand Manan</t>
+  </si>
+  <si>
+    <t>Grande-Anse</t>
   </si>
   <si>
     <t>Hampton</t>
@@ -2162,80 +2165,80 @@
         <v>48</v>
       </c>
       <c r="B38" s="3">
-        <v>102569700</v>
+        <v>103165300</v>
       </c>
       <c r="C38" s="3">
-        <v>457100</v>
+        <v>552000</v>
       </c>
       <c r="D38" s="3">
-        <v>5542700</v>
+        <v>5635600</v>
       </c>
       <c r="E38" s="3">
-        <v>108569500</v>
+        <v>109352900</v>
       </c>
       <c r="F38" s="3">
         <v>15022300</v>
       </c>
       <c r="G38" s="3">
-        <v>799400</v>
+        <v>866300</v>
       </c>
       <c r="H38" s="3">
         <v>1690700</v>
       </c>
       <c r="I38" s="3">
-        <v>17512400</v>
+        <v>17579300</v>
       </c>
       <c r="J38" s="3">
-        <v>126081900</v>
+        <v>126932200</v>
       </c>
       <c r="K38" s="3">
-        <v>134838100</v>
+        <v>135721850</v>
       </c>
       <c r="L38" s="3">
-        <v>134799014</v>
+        <v>135682764</v>
       </c>
     </row>
     <row r="39" spans="1:12">
       <c r="A39" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B39" s="3">
-        <v>20854200</v>
+        <v>20258600</v>
       </c>
       <c r="C39" s="3">
-        <v>94900</v>
+        <v>0</v>
       </c>
       <c r="D39" s="3">
-        <v>3699600</v>
+        <v>3606700</v>
       </c>
       <c r="E39" s="3">
-        <v>24648700</v>
+        <v>23865300</v>
       </c>
       <c r="F39" s="3">
         <v>4262700</v>
       </c>
       <c r="G39" s="3">
-        <v>149200</v>
+        <v>82300</v>
       </c>
       <c r="H39" s="3">
         <v>472300</v>
       </c>
       <c r="I39" s="3">
-        <v>4884200</v>
+        <v>4817300</v>
       </c>
       <c r="J39" s="3">
-        <v>29532900</v>
+        <v>28682600</v>
       </c>
       <c r="K39" s="3">
-        <v>31975000</v>
+        <v>31091250</v>
       </c>
       <c r="L39" s="3">
-        <v>31954125</v>
+        <v>31070375</v>
       </c>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B40" s="3">
         <v>142080300</v>
@@ -2273,7 +2276,7 @@
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B41" s="3">
         <v>26392400</v>
@@ -2311,7 +2314,7 @@
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B42" s="3">
         <v>37945600</v>
@@ -2349,7 +2352,7 @@
     </row>
     <row r="43" spans="1:12">
       <c r="A43" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B43" s="3">
         <v>24417400</v>
@@ -2387,7 +2390,7 @@
     </row>
     <row r="44" spans="1:12">
       <c r="A44" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B44" s="3">
         <v>33203600</v>
@@ -2425,7 +2428,7 @@
     </row>
     <row r="45" spans="1:12">
       <c r="A45" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B45" s="3">
         <v>21556100</v>
@@ -2463,7 +2466,7 @@
     </row>
     <row r="46" spans="1:12">
       <c r="A46" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B46" s="3">
         <v>130492400</v>
@@ -2501,7 +2504,7 @@
     </row>
     <row r="47" spans="1:12">
       <c r="A47" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B47" s="3">
         <v>57945300</v>
@@ -2539,7 +2542,7 @@
     </row>
     <row r="48" spans="1:12">
       <c r="A48" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B48" s="3">
         <v>28916400</v>
@@ -2577,7 +2580,7 @@
     </row>
     <row r="49" spans="1:12">
       <c r="A49" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B49" s="3">
         <v>42213000</v>
@@ -2615,7 +2618,7 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B50" s="3">
         <v>47762400</v>
@@ -2653,7 +2656,7 @@
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B51" s="3">
         <v>46473600</v>
@@ -2691,7 +2694,7 @@
     </row>
     <row r="52" spans="1:12">
       <c r="A52" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B52" s="3">
         <v>41965500</v>
@@ -2729,7 +2732,7 @@
     </row>
     <row r="53" spans="1:12">
       <c r="A53" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B53" s="3">
         <v>26955300</v>
@@ -2767,7 +2770,7 @@
     </row>
     <row r="54" spans="1:12">
       <c r="A54" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B54" s="3">
         <v>23770100</v>
@@ -2805,7 +2808,7 @@
     </row>
     <row r="55" spans="1:12">
       <c r="A55" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B55" s="3">
         <v>33715300</v>
@@ -2843,7 +2846,7 @@
     </row>
     <row r="56" spans="1:12">
       <c r="A56" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B56" s="3">
         <v>25508900</v>
@@ -2881,7 +2884,7 @@
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B57" s="3">
         <v>132037800</v>
@@ -2919,7 +2922,7 @@
     </row>
     <row r="58" spans="1:12">
       <c r="A58" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B58" s="3">
         <v>46010100</v>
@@ -2957,7 +2960,7 @@
     </row>
     <row r="59" spans="1:12">
       <c r="A59" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B59" s="3">
         <v>45327100</v>
@@ -2995,7 +2998,7 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B60" s="3">
         <v>18617500</v>
@@ -3033,7 +3036,7 @@
     </row>
     <row r="61" spans="1:12">
       <c r="A61" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B61" s="3">
         <v>59922300</v>
@@ -3071,7 +3074,7 @@
     </row>
     <row r="62" spans="1:12">
       <c r="A62" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B62" s="3">
         <v>64736100</v>
@@ -3109,7 +3112,7 @@
     </row>
     <row r="63" spans="1:12">
       <c r="A63" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B63" s="3">
         <v>34818000</v>
@@ -3147,7 +3150,7 @@
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B64" s="3">
         <v>13574300</v>
@@ -3185,7 +3188,7 @@
     </row>
     <row r="65" spans="1:12">
       <c r="A65" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B65" s="3">
         <v>7648900</v>
@@ -3223,7 +3226,7 @@
     </row>
     <row r="66" spans="1:12">
       <c r="A66" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B66" s="3">
         <v>14197600</v>
@@ -3261,7 +3264,7 @@
     </row>
     <row r="67" spans="1:12">
       <c r="A67" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B67" s="3">
         <v>41395200</v>
@@ -3299,7 +3302,7 @@
     </row>
     <row r="68" spans="1:12">
       <c r="A68" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B68" s="3">
         <v>31393000</v>
@@ -3337,7 +3340,7 @@
     </row>
     <row r="69" spans="1:12">
       <c r="A69" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B69" s="3">
         <v>11806400</v>
@@ -3375,7 +3378,7 @@
     </row>
     <row r="70" spans="1:12">
       <c r="A70" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B70" s="3">
         <v>27515100</v>
@@ -3413,7 +3416,7 @@
     </row>
     <row r="71" spans="1:12">
       <c r="A71" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B71" s="3">
         <v>22710300</v>
@@ -3451,7 +3454,7 @@
     </row>
     <row r="72" spans="1:12">
       <c r="A72" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B72" s="3">
         <v>19967800</v>
@@ -3489,7 +3492,7 @@
     </row>
     <row r="73" spans="1:12">
       <c r="A73" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B73" s="3">
         <v>43395800</v>
@@ -3527,7 +3530,7 @@
     </row>
     <row r="74" spans="1:12">
       <c r="A74" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B74" s="3">
         <v>6374500</v>
@@ -3565,7 +3568,7 @@
     </row>
     <row r="75" spans="1:12">
       <c r="A75" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B75" s="3">
         <v>13215800</v>
@@ -3603,7 +3606,7 @@
     </row>
     <row r="76" spans="1:12">
       <c r="A76" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B76" s="3">
         <v>9574800</v>
@@ -3641,7 +3644,7 @@
     </row>
     <row r="77" spans="1:12">
       <c r="A77" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B77" s="3">
         <v>28808800</v>
@@ -3679,7 +3682,7 @@
     </row>
     <row r="78" spans="1:12">
       <c r="A78" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B78" s="3">
         <v>19131700</v>
@@ -3717,7 +3720,7 @@
     </row>
     <row r="79" spans="1:12">
       <c r="A79" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B79" s="3">
         <v>31099900</v>
@@ -3755,7 +3758,7 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B80" s="3">
         <v>9147900</v>
@@ -3793,7 +3796,7 @@
     </row>
     <row r="81" spans="1:12">
       <c r="A81" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B81" s="3">
         <v>14673900</v>
@@ -3831,7 +3834,7 @@
     </row>
     <row r="82" spans="1:12">
       <c r="A82" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B82" s="3">
         <v>15249100</v>
@@ -3869,7 +3872,7 @@
     </row>
     <row r="83" spans="1:12">
       <c r="A83" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B83" s="3">
         <v>5182200</v>
@@ -3907,7 +3910,7 @@
     </row>
     <row r="84" spans="1:12">
       <c r="A84" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B84" s="3">
         <v>6990900</v>
@@ -3945,7 +3948,7 @@
     </row>
     <row r="85" spans="1:12">
       <c r="A85" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B85" s="3">
         <v>21640300</v>
@@ -3983,7 +3986,7 @@
     </row>
     <row r="86" spans="1:12">
       <c r="A86" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B86" s="3">
         <v>36429400</v>
@@ -4021,7 +4024,7 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B87" s="3">
         <v>14790300</v>
@@ -4059,7 +4062,7 @@
     </row>
     <row r="88" spans="1:12">
       <c r="A88" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" s="3">
         <v>20686000</v>
@@ -4097,7 +4100,7 @@
     </row>
     <row r="89" spans="1:12">
       <c r="A89" s="2" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B89" s="3">
         <v>9285800</v>
@@ -4135,7 +4138,7 @@
     </row>
     <row r="90" spans="1:12">
       <c r="A90" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B90" s="3">
         <v>9188300</v>
@@ -4173,7 +4176,7 @@
     </row>
     <row r="91" spans="1:12">
       <c r="A91" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B91" s="3">
         <v>20072200</v>
@@ -4211,7 +4214,7 @@
     </row>
     <row r="92" spans="1:12">
       <c r="A92" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B92" s="3">
         <v>14199500</v>
@@ -4249,7 +4252,7 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B93" s="3">
         <v>19671000</v>
@@ -4287,7 +4290,7 @@
     </row>
     <row r="94" spans="1:12">
       <c r="A94" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B94" s="3">
         <v>12153000</v>
@@ -4325,7 +4328,7 @@
     </row>
     <row r="95" spans="1:12">
       <c r="A95" s="2" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B95" s="3">
         <v>25666100</v>
@@ -4363,7 +4366,7 @@
     </row>
     <row r="96" spans="1:12">
       <c r="A96" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B96" s="3">
         <v>18864600</v>
@@ -4401,7 +4404,7 @@
     </row>
     <row r="97" spans="1:12">
       <c r="A97" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B97" s="3">
         <v>12960100</v>
@@ -4439,7 +4442,7 @@
     </row>
     <row r="98" spans="1:12">
       <c r="A98" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B98" s="3">
         <v>5968300</v>
@@ -4477,7 +4480,7 @@
     </row>
     <row r="99" spans="1:12">
       <c r="A99" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B99" s="3">
         <v>11399000</v>
@@ -4515,7 +4518,7 @@
     </row>
     <row r="100" spans="1:12">
       <c r="A100" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B100" s="3">
         <v>11074900</v>
@@ -4553,7 +4556,7 @@
     </row>
     <row r="101" spans="1:12">
       <c r="A101" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B101" s="3">
         <v>45862600</v>
@@ -4591,7 +4594,7 @@
     </row>
     <row r="102" spans="1:12">
       <c r="A102" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B102" s="3">
         <v>35327900</v>
@@ -4629,7 +4632,7 @@
     </row>
     <row r="103" spans="1:12">
       <c r="A103" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B103" s="3">
         <v>15334900</v>
@@ -4667,7 +4670,7 @@
     </row>
     <row r="104" spans="1:12">
       <c r="A104" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B104" s="3">
         <v>4537900</v>

</xml_diff>